<commit_message>
Updates to HYP assay recipe sheets
Added new columns with calculations for additional final volumes of each recipe
</commit_message>
<xml_diff>
--- a/Biochemistry/Hydroxyproline Assay/RecipeSheets/ElrichsReagent_soln_recipe.xlsx
+++ b/Biochemistry/Hydroxyproline Assay/RecipeSheets/ElrichsReagent_soln_recipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\GitHub\Protocols\Biochemistry\Hydroxyproline Assay\RecipeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBE277B-9DDF-4569-B072-362DC3FE3421}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AACBECF-CF64-4097-AA04-9358D75E987E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -806,17 +806,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1407,10 +1407,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="70"/>
+      <c r="B1" s="72"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1506,10 +1506,10 @@
       <c r="L7" s="33"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="70"/>
+      <c r="B8" s="72"/>
       <c r="L8" s="33"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1637,10 +1637,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="70"/>
+      <c r="B1" s="72"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1832,10 +1832,10 @@
       <c r="O9" s="47"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="70"/>
+      <c r="B10" s="72"/>
       <c r="M10" s="49">
         <f>(N6+N8)</f>
         <v>63.428571428571431</v>
@@ -1915,7 +1915,7 @@
         <v>52</v>
       </c>
       <c r="O13" s="53">
-        <f t="shared" ref="O13:O15" si="3">N13*$M$11</f>
+        <f t="shared" ref="O13:O14" si="3">N13*$M$11</f>
         <v>40.990990990990987</v>
       </c>
       <c r="P13" s="54"/>
@@ -2043,7 +2043,7 @@
       <c r="N17" s="50">
         <v>16</v>
       </c>
-      <c r="O17" s="71" t="s">
+      <c r="O17" s="69" t="s">
         <v>42</v>
       </c>
       <c r="P17" s="51">
@@ -2066,7 +2066,7 @@
         <f>(P17*0.5)/0.7</f>
         <v>1.6806722689075633</v>
       </c>
-      <c r="Q18" s="72"/>
+      <c r="Q18" s="70"/>
     </row>
     <row r="19" spans="1:17" ht="38.25" x14ac:dyDescent="0.2">
       <c r="H19" s="46"/>
@@ -2122,21 +2122,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100965EA08FA511AE4C9FFF632E6536ED13" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abfa450e2c882fa05ec7f6a4b4016779">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a" xmlns:ns3="6cbc0c5a-d948-46e5-8624-1bad210f77c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53678093842f3275b6926b32e7a9c141" ns2:_="" ns3:_="">
     <xsd:import namespace="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
@@ -2359,32 +2344,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33AFEA7C-ECB0-4A51-9E17-02E120CDEEE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
-    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A161E6A-5B3F-4912-ADEE-71AD0FF6FC00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2401,4 +2376,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33AFEA7C-ECB0-4A51-9E17-02E120CDEEE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
+    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to Elrich's Reagent recipe sheet and Added new SOP updated version
Minor update to units for one of the components of Elrich's reagents. Updated the HYP Assay SOP and added the newly updated version to GitHub
</commit_message>
<xml_diff>
--- a/Biochemistry/Hydroxyproline Assay/RecipeSheets/ElrichsReagent_soln_recipe.xlsx
+++ b/Biochemistry/Hydroxyproline Assay/RecipeSheets/ElrichsReagent_soln_recipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\GitHub\Protocols\Biochemistry\Hydroxyproline Assay\RecipeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402EB9EF-F12C-47F3-B84C-6C2B9B16D9E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3AD57E-ECB4-4ED9-AE18-3747687A4B93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -197,14 +197,14 @@
     <t>Units</t>
   </si>
   <si>
-    <t>mg</t>
-  </si>
-  <si>
     <t>mL</t>
   </si>
   <si>
     <t>Amount for
 15mL</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1713,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1780,7 +1780,7 @@
         <v>32</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4" s="43" t="s">
         <v>33</v>
@@ -1814,7 +1814,7 @@
       <c r="J5" s="38"/>
       <c r="K5" s="38"/>
       <c r="L5" s="71" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M5" s="39"/>
       <c r="O5" s="52" t="s">
@@ -1844,7 +1844,7 @@
       <c r="J6" s="38"/>
       <c r="K6" s="38"/>
       <c r="L6" s="72" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M6" s="31"/>
       <c r="O6" s="52" t="s">
@@ -1874,7 +1874,7 @@
       <c r="J7" s="23"/>
       <c r="K7" s="23"/>
       <c r="L7" s="73" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M7" s="9"/>
       <c r="O7" s="55" t="s">
@@ -1996,7 +1996,7 @@
         <v>32</v>
       </c>
       <c r="J13" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K13" s="43" t="s">
         <v>33</v>
@@ -2045,7 +2045,7 @@
         <v>0.88235294117647056</v>
       </c>
       <c r="L14" s="71" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M14" s="39"/>
       <c r="O14" s="55" t="s">
@@ -2075,7 +2075,7 @@
         <v>38.235294117647058</v>
       </c>
       <c r="I15" s="38">
-        <f t="shared" ref="I14:I17" si="3">K15*2.5</f>
+        <f t="shared" ref="I15:I17" si="3">K15*2.5</f>
         <v>19.117647058823529</v>
       </c>
       <c r="J15" s="38">
@@ -2086,7 +2086,7 @@
         <v>7.6470588235294121</v>
       </c>
       <c r="L15" s="72" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M15" s="31"/>
       <c r="O15" s="62" t="s">
@@ -2131,7 +2131,7 @@
         <v>0.67226890756302504</v>
       </c>
       <c r="L16" s="74" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M16" s="7"/>
     </row>
@@ -2161,7 +2161,7 @@
         <v>1.6806722689075633</v>
       </c>
       <c r="L17" s="73" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M17" s="9"/>
       <c r="O17" s="64" t="s">
@@ -2249,6 +2249,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100965EA08FA511AE4C9FFF632E6536ED13" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abfa450e2c882fa05ec7f6a4b4016779">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a" xmlns:ns3="6cbc0c5a-d948-46e5-8624-1bad210f77c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53678093842f3275b6926b32e7a9c141" ns2:_="" ns3:_="">
     <xsd:import namespace="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
@@ -2471,22 +2486,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33AFEA7C-ECB0-4A51-9E17-02E120CDEEE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
+    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A161E6A-5B3F-4912-ADEE-71AD0FF6FC00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2503,29 +2528,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33AFEA7C-ECB0-4A51-9E17-02E120CDEEE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
-    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Minor changes to HYP Assay recipe sheets
Basically just formatting edits to make printout more convenient to write on and easier to see text
</commit_message>
<xml_diff>
--- a/Biochemistry/Hydroxyproline Assay/RecipeSheets/ElrichsReagent_soln_recipe.xlsx
+++ b/Biochemistry/Hydroxyproline Assay/RecipeSheets/ElrichsReagent_soln_recipe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\GitHub\Protocols\Biochemistry\Hydroxyproline Assay\RecipeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3AD57E-ECB4-4ED9-AE18-3747687A4B93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A325ECF8-C0C5-4C2F-BF18-AA160E6D3368}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1020,16 +1020,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1044,7 +1044,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2324100" y="161925"/>
+          <a:off x="5400675" y="152400"/>
           <a:ext cx="2266950" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1100,16 +1100,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1124,7 +1124,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2333625" y="2857500"/>
+          <a:off x="5419725" y="2867025"/>
           <a:ext cx="2266950" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1713,18 +1713,18 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="A10" sqref="A10:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="9" max="11" width="10.85546875" customWidth="1"/>
     <col min="12" max="12" width="4.7109375" customWidth="1"/>
@@ -2242,28 +2242,13 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A10:B10"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="91" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100965EA08FA511AE4C9FFF632E6536ED13" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abfa450e2c882fa05ec7f6a4b4016779">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a" xmlns:ns3="6cbc0c5a-d948-46e5-8624-1bad210f77c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53678093842f3275b6926b32e7a9c141" ns2:_="" ns3:_="">
     <xsd:import namespace="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
@@ -2486,32 +2471,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33AFEA7C-ECB0-4A51-9E17-02E120CDEEE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
-    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A161E6A-5B3F-4912-ADEE-71AD0FF6FC00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2528,4 +2503,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33AFEA7C-ECB0-4A51-9E17-02E120CDEEE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
+    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>